<commit_message>
added mi8 to CF file and updated Mi8 freqs
</commit_message>
<xml_diff>
--- a/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
+++ b/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ECAEED-EC89-46A8-9E2D-4B8E5F4BA6BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFEA301-B7C0-45CF-B1BF-37F61845C18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35805" yWindow="2910" windowWidth="21600" windowHeight="12975" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35940" yWindow="6930" windowWidth="21600" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1695" uniqueCount="765">
   <si>
     <t>AWACS</t>
   </si>
@@ -1747,9 +1747,6 @@
     <t>RW internal #6</t>
   </si>
   <si>
-    <t>KA-50 presets OPUF V1.0</t>
-  </si>
-  <si>
     <t>11y</t>
   </si>
   <si>
@@ -1960,9 +1957,6 @@
     <t>Internal #10</t>
   </si>
   <si>
-    <t xml:space="preserve">A-10C presets  - OPUF v 1.0 </t>
-  </si>
-  <si>
     <t>MAROON 11</t>
   </si>
   <si>
@@ -2318,6 +2312,15 @@
   </si>
   <si>
     <t>MI-8 presets OPBH V1.0</t>
+  </si>
+  <si>
+    <t>G Washington ATIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A-10C presets  - OPBH v 1.0 </t>
+  </si>
+  <si>
+    <t>KA-50 presets OPBH V1.0</t>
   </si>
 </sst>
 </file>
@@ -3462,138 +3465,6 @@
     <xf numFmtId="0" fontId="16" fillId="19" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="19" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3606,6 +3477,138 @@
     </xf>
     <xf numFmtId="49" fontId="22" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3947,8 +3950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:AF51"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O51" sqref="O51"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4044,21 +4047,21 @@
       <c r="S4" s="30" t="s">
         <v>540</v>
       </c>
-      <c r="V4" s="130" t="s">
+      <c r="V4" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="130"/>
-      <c r="X4" s="130"/>
-      <c r="Z4" s="130" t="s">
+      <c r="W4" s="136"/>
+      <c r="X4" s="136"/>
+      <c r="Z4" s="136" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" s="130"/>
-      <c r="AB4" s="130"/>
-      <c r="AD4" s="130" t="s">
+      <c r="AA4" s="136"/>
+      <c r="AB4" s="136"/>
+      <c r="AD4" s="136" t="s">
         <v>293</v>
       </c>
-      <c r="AE4" s="130"/>
-      <c r="AF4" s="130"/>
+      <c r="AE4" s="136"/>
+      <c r="AF4" s="136"/>
     </row>
     <row r="5" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="51" t="s">
@@ -4284,13 +4287,13 @@
         <v>551</v>
       </c>
       <c r="AD7" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="AE7" s="12" t="s">
         <v>138</v>
       </c>
       <c r="AF7" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="8" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
@@ -4537,11 +4540,11 @@
       <c r="X11" t="s">
         <v>510</v>
       </c>
-      <c r="Z11" s="130" t="s">
+      <c r="Z11" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="AA11" s="130"/>
-      <c r="AB11" s="130"/>
+      <c r="AA11" s="136"/>
+      <c r="AB11" s="136"/>
     </row>
     <row r="12" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="51" t="s">
@@ -4793,10 +4796,10 @@
       </c>
       <c r="Q15" s="4"/>
       <c r="R15" s="82" t="s">
+        <v>616</v>
+      </c>
+      <c r="S15" s="83" t="s">
         <v>617</v>
-      </c>
-      <c r="S15" s="83" t="s">
-        <v>618</v>
       </c>
       <c r="V15" s="8" t="s">
         <v>13</v>
@@ -4859,13 +4862,13 @@
       </c>
       <c r="Q16" s="4"/>
       <c r="R16" s="84" t="s">
+        <v>614</v>
+      </c>
+      <c r="S16" s="85" t="s">
         <v>615</v>
       </c>
-      <c r="S16" s="85" t="s">
-        <v>616</v>
-      </c>
       <c r="V16" s="67" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="W16" s="68">
         <v>301</v>
@@ -4917,7 +4920,7 @@
       </c>
       <c r="Q17" s="4"/>
       <c r="V17" s="67" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="W17">
         <v>300</v>
@@ -4968,11 +4971,11 @@
         <v>311</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="130" t="s">
+      <c r="R18" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="S18" s="130"/>
-      <c r="T18" s="130"/>
+      <c r="S18" s="136"/>
+      <c r="T18" s="136"/>
     </row>
     <row r="19" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B19" s="51" t="s">
@@ -5028,20 +5031,20 @@
       <c r="T19" s="45" t="s">
         <v>302</v>
       </c>
-      <c r="V19" s="132" t="s">
+      <c r="V19" s="137" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="133"/>
-      <c r="X19" s="133"/>
-      <c r="Y19" s="133"/>
-      <c r="Z19" s="134"/>
-      <c r="AB19" s="130" t="s">
+      <c r="W19" s="138"/>
+      <c r="X19" s="138"/>
+      <c r="Y19" s="138"/>
+      <c r="Z19" s="139"/>
+      <c r="AB19" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="AC19" s="130"/>
-      <c r="AD19" s="130"/>
-      <c r="AE19" s="130"/>
-      <c r="AF19" s="130"/>
+      <c r="AC19" s="136"/>
+      <c r="AD19" s="136"/>
+      <c r="AE19" s="136"/>
+      <c r="AF19" s="136"/>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B20" s="51" t="s">
@@ -5098,7 +5101,7 @@
         <v>533</v>
       </c>
       <c r="U20" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="V20" s="45" t="s">
         <v>302</v>
@@ -5181,7 +5184,7 @@
         <v>534</v>
       </c>
       <c r="U21" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="V21" s="4" t="s">
         <v>531</v>
@@ -5190,13 +5193,13 @@
         <v>104</v>
       </c>
       <c r="X21" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="Y21" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="Y21" s="4" t="s">
-        <v>625</v>
-      </c>
       <c r="AB21" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="AC21" s="9" t="s">
         <v>58</v>
@@ -5259,16 +5262,16 @@
         <v>532</v>
       </c>
       <c r="W22" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="Y22" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="Z22" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="AB22" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="AC22" s="9" t="s">
         <v>269</v>
@@ -5328,13 +5331,13 @@
         <v>403</v>
       </c>
       <c r="AB23" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="AC23" s="9" t="s">
         <v>94</v>
       </c>
       <c r="AD23" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="AE23" s="9" t="s">
         <v>167</v>
@@ -5430,11 +5433,11 @@
       </c>
       <c r="O25" s="46"/>
       <c r="P25" s="4"/>
-      <c r="R25" s="130" t="s">
+      <c r="R25" s="136" t="s">
         <v>556</v>
       </c>
-      <c r="S25" s="130"/>
-      <c r="T25" s="130"/>
+      <c r="S25" s="136"/>
+      <c r="T25" s="136"/>
     </row>
     <row r="26" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B26" s="51" t="s">
@@ -5531,13 +5534,13 @@
       </c>
       <c r="O27" s="46"/>
       <c r="R27" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="S27" t="s">
         <v>557</v>
       </c>
       <c r="U27" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="28" spans="2:32" x14ac:dyDescent="0.25">
@@ -5575,43 +5578,51 @@
         <v>11</v>
       </c>
       <c r="R28" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="S28" t="s">
         <v>558</v>
       </c>
       <c r="U28" t="s">
-        <v>746</v>
+        <v>744</v>
+      </c>
+    </row>
+    <row r="29" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="R29" t="s">
+        <v>762</v>
+      </c>
+      <c r="S29">
+        <v>280.60000000000002</v>
       </c>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B31" s="130" t="s">
+      <c r="B31" s="136" t="s">
         <v>312</v>
       </c>
-      <c r="C31" s="130"/>
-      <c r="D31" s="130"/>
-      <c r="E31" s="130"/>
-      <c r="F31" s="130"/>
-      <c r="G31" s="130"/>
-      <c r="H31" s="130"/>
-      <c r="J31" s="130" t="s">
+      <c r="C31" s="136"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="136"/>
+      <c r="H31" s="136"/>
+      <c r="J31" s="136" t="s">
         <v>313</v>
       </c>
-      <c r="K31" s="130"/>
-      <c r="L31" s="130"/>
-      <c r="M31" s="130"/>
-      <c r="N31" s="130"/>
-      <c r="O31" s="130"/>
-      <c r="P31" s="130"/>
-      <c r="U31" s="130" t="s">
+      <c r="K31" s="136"/>
+      <c r="L31" s="136"/>
+      <c r="M31" s="136"/>
+      <c r="N31" s="136"/>
+      <c r="O31" s="136"/>
+      <c r="P31" s="136"/>
+      <c r="U31" s="136" t="s">
         <v>295</v>
       </c>
-      <c r="V31" s="130"/>
-      <c r="W31" s="130"/>
-      <c r="X31" s="130"/>
-      <c r="Y31" s="130"/>
-      <c r="Z31" s="130"/>
-      <c r="AA31" s="130"/>
+      <c r="V31" s="136"/>
+      <c r="W31" s="136"/>
+      <c r="X31" s="136"/>
+      <c r="Y31" s="136"/>
+      <c r="Z31" s="136"/>
+      <c r="AA31" s="136"/>
     </row>
     <row r="32" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B32" s="45" t="s">
@@ -5725,7 +5736,7 @@
         <v>426</v>
       </c>
       <c r="V33" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="W33" t="s">
         <v>417</v>
@@ -5740,7 +5751,7 @@
         <v>260</v>
       </c>
       <c r="AA33" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
     </row>
     <row r="34" spans="2:27" x14ac:dyDescent="0.25">
@@ -5790,7 +5801,7 @@
         <v>435</v>
       </c>
       <c r="V34" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="W34" t="s">
         <v>417</v>
@@ -5805,7 +5816,7 @@
         <v>141</v>
       </c>
       <c r="AA34" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
     </row>
     <row r="35" spans="2:27" x14ac:dyDescent="0.25">
@@ -5855,7 +5866,7 @@
         <v>441</v>
       </c>
       <c r="V35" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="W35" t="s">
         <v>417</v>
@@ -5870,7 +5881,7 @@
         <v>235</v>
       </c>
       <c r="AA35" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="36" spans="2:27" x14ac:dyDescent="0.25">
@@ -5878,7 +5889,7 @@
         <v>436</v>
       </c>
       <c r="C36" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D36" t="s">
         <v>467</v>
@@ -5920,7 +5931,7 @@
         <v>445</v>
       </c>
       <c r="V36" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="W36" t="s">
         <v>417</v>
@@ -5935,7 +5946,7 @@
         <v>247</v>
       </c>
       <c r="AA36" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="37" spans="2:27" x14ac:dyDescent="0.25">
@@ -5943,7 +5954,7 @@
         <v>438</v>
       </c>
       <c r="C37" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="D37" t="s">
         <v>467</v>
@@ -5985,7 +5996,7 @@
         <v>449</v>
       </c>
       <c r="V37" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="W37" t="s">
         <v>417</v>
@@ -6000,7 +6011,7 @@
         <v>163</v>
       </c>
       <c r="AA37" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="38" spans="2:27" x14ac:dyDescent="0.25">
@@ -6008,7 +6019,7 @@
         <v>204</v>
       </c>
       <c r="F38" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="J38" t="s">
         <v>430</v>
@@ -6035,7 +6046,7 @@
         <v>447</v>
       </c>
       <c r="V38" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="W38" t="s">
         <v>417</v>
@@ -6050,7 +6061,7 @@
         <v>151</v>
       </c>
       <c r="AA38" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="39" spans="2:27" x14ac:dyDescent="0.25">
@@ -6058,25 +6069,25 @@
         <v>230</v>
       </c>
       <c r="F39" t="s">
-        <v>635</v>
-      </c>
-      <c r="J39" s="131" t="s">
+        <v>634</v>
+      </c>
+      <c r="J39" s="135" t="s">
         <v>493</v>
       </c>
-      <c r="K39" s="131"/>
-      <c r="L39" s="131"/>
-      <c r="M39" s="131"/>
-      <c r="N39" s="131"/>
-      <c r="O39" s="131"/>
-      <c r="P39" s="131"/>
+      <c r="K39" s="135"/>
+      <c r="L39" s="135"/>
+      <c r="M39" s="135"/>
+      <c r="N39" s="135"/>
+      <c r="O39" s="135"/>
+      <c r="P39" s="135"/>
       <c r="T39">
         <v>7</v>
       </c>
       <c r="U39" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="V39" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="W39" t="s">
         <v>417</v>
@@ -6091,7 +6102,7 @@
         <v>220</v>
       </c>
       <c r="AA39" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
     </row>
     <row r="40" spans="2:27" x14ac:dyDescent="0.25">
@@ -6099,16 +6110,16 @@
         <v>255</v>
       </c>
       <c r="F40" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="T40">
         <v>8</v>
       </c>
       <c r="U40" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="V40" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="W40" t="s">
         <v>417</v>
@@ -6123,7 +6134,7 @@
         <v>276</v>
       </c>
       <c r="AA40" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="41" spans="2:27" x14ac:dyDescent="0.25">
@@ -6131,16 +6142,16 @@
         <v>254</v>
       </c>
       <c r="F41" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="T41">
         <v>9</v>
       </c>
       <c r="U41" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="V41" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="W41" t="s">
         <v>417</v>
@@ -6155,7 +6166,7 @@
         <v>219</v>
       </c>
       <c r="AA41" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="42" spans="2:27" x14ac:dyDescent="0.25">
@@ -6163,7 +6174,7 @@
         <v>177</v>
       </c>
       <c r="F42" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="T42">
         <v>10</v>
@@ -6181,121 +6192,116 @@
         <v>253</v>
       </c>
       <c r="AA42" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="44" spans="2:27" x14ac:dyDescent="0.25">
       <c r="U44" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="W44" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="X44" s="16" t="s">
         <v>84</v>
       </c>
       <c r="Y44" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="Z44" s="17" t="s">
         <v>145</v>
       </c>
       <c r="AA44" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="45" spans="2:27" x14ac:dyDescent="0.25">
       <c r="W45" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="X45" s="16" t="s">
         <v>137</v>
       </c>
       <c r="Y45" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="Z45" s="17" t="s">
         <v>70</v>
       </c>
       <c r="AA45" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
     </row>
     <row r="46" spans="2:27" x14ac:dyDescent="0.25">
       <c r="W46" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="X46" s="16" t="s">
         <v>115</v>
       </c>
       <c r="Y46" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="Z46" s="17" t="s">
         <v>205</v>
       </c>
       <c r="AA46" s="2" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
     </row>
     <row r="49" spans="23:27" x14ac:dyDescent="0.25">
       <c r="W49" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="X49" s="16" t="s">
         <v>100</v>
       </c>
       <c r="Y49" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="Z49" s="17" t="s">
         <v>124</v>
       </c>
       <c r="AA49" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
     </row>
     <row r="50" spans="23:27" x14ac:dyDescent="0.25">
       <c r="W50" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="X50" s="16" t="s">
         <v>158</v>
       </c>
       <c r="Y50" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="Z50" s="17" t="s">
         <v>136</v>
       </c>
       <c r="AA50" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
     </row>
     <row r="51" spans="23:27" x14ac:dyDescent="0.25">
       <c r="W51" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="X51" s="16" t="s">
         <v>74</v>
       </c>
       <c r="Y51" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="Z51" s="17" t="s">
         <v>150</v>
       </c>
       <c r="AA51" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="U31:AA31"/>
-    <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="V19:Z19"/>
-    <mergeCell ref="J31:P31"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="R18:T18"/>
     <mergeCell ref="AB19:AF19"/>
@@ -6303,6 +6309,11 @@
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="R25:T25"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="U31:AA31"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="V19:Z19"/>
+    <mergeCell ref="J31:P31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -6328,34 +6339,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="169" t="s">
+      <c r="A1" s="175" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="169"/>
-      <c r="C1" s="169"/>
-      <c r="D1" s="169"/>
-      <c r="E1" s="169"/>
-      <c r="F1" s="169"/>
+      <c r="B1" s="175"/>
+      <c r="C1" s="175"/>
+      <c r="D1" s="175"/>
+      <c r="E1" s="175"/>
+      <c r="F1" s="175"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="170"/>
-      <c r="B2" s="170"/>
-      <c r="C2" s="170"/>
-      <c r="D2" s="170"/>
-      <c r="E2" s="170"/>
-      <c r="F2" s="170"/>
+      <c r="A2" s="176"/>
+      <c r="B2" s="176"/>
+      <c r="C2" s="176"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="143" t="s">
         <v>333</v>
       </c>
-      <c r="B3" s="139"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="138" t="s">
+      <c r="B3" s="144"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="143" t="s">
         <v>334</v>
       </c>
-      <c r="E3" s="139"/>
-      <c r="F3" s="140"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="145"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="48">
@@ -6897,22 +6908,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="171" t="s">
+      <c r="A1" s="177" t="s">
         <v>376</v>
       </c>
-      <c r="B1" s="171"/>
-      <c r="C1" s="171"/>
-      <c r="D1" s="171"/>
-      <c r="E1" s="171"/>
-      <c r="F1" s="171"/>
+      <c r="B1" s="177"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
     </row>
     <row r="2" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="172" t="s">
+      <c r="B2" s="178" t="s">
         <v>377</v>
       </c>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
+      <c r="C2" s="178"/>
+      <c r="D2" s="178"/>
+      <c r="E2" s="178"/>
     </row>
     <row r="3" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="38"/>
@@ -7017,12 +7028,12 @@
       <c r="E10" s="38"/>
     </row>
     <row r="14" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B14" s="172" t="s">
+      <c r="B14" s="178" t="s">
         <v>394</v>
       </c>
-      <c r="C14" s="172"/>
-      <c r="D14" s="172"/>
-      <c r="E14" s="172"/>
+      <c r="C14" s="178"/>
+      <c r="D14" s="178"/>
+      <c r="E14" s="178"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B15" s="38"/>
@@ -7147,257 +7158,257 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B1" s="32">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H1" s="32">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N1" s="32">
         <v>1</v>
       </c>
       <c r="O1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B2" s="32">
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G2" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H2" s="32">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M2" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N2" s="32">
         <v>2</v>
       </c>
       <c r="O2" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B3" s="32">
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G3" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H3" s="32">
         <v>3</v>
       </c>
       <c r="I3" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M3" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N3" s="32">
         <v>3</v>
       </c>
       <c r="O3" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B4" s="32">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G4" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H4" s="32">
         <v>4</v>
       </c>
       <c r="I4" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M4" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N4" s="32">
         <v>4</v>
       </c>
       <c r="O4" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B5" s="32">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G5" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H5" s="32">
         <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M5" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N5" s="32">
         <v>5</v>
       </c>
       <c r="O5" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B6" s="32">
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G6" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H6" s="32">
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M6" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N6" s="32">
         <v>6</v>
       </c>
       <c r="O6" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B7" s="32">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G7" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H7" s="32">
         <v>7</v>
       </c>
       <c r="I7" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M7" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N7" s="32">
         <v>7</v>
       </c>
       <c r="O7" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B8" s="32">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G8" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H8" s="32">
         <v>8</v>
       </c>
       <c r="I8" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M8" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N8" s="32">
         <v>8</v>
       </c>
       <c r="O8" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="B9" s="32">
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G9" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="H9" s="32">
         <v>9</v>
       </c>
       <c r="I9" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M9" s="3" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="N9" s="69">
         <v>9</v>
@@ -7406,542 +7417,542 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B11" s="32">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G11" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H11" s="32">
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M11" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N11" s="32">
         <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B12" s="32">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G12" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H12" s="32">
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M12" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N12" s="32">
         <v>2</v>
       </c>
       <c r="O12" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B13" s="32">
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G13" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H13" s="32">
         <v>3</v>
       </c>
       <c r="I13" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="M13" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N13" s="32">
         <v>3</v>
       </c>
       <c r="O13" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B14" s="32">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G14" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H14" s="32">
         <v>4</v>
       </c>
       <c r="I14" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="M14" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N14" s="32">
         <v>4</v>
       </c>
       <c r="O14" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B15" s="32">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G15" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H15" s="32">
         <v>5</v>
       </c>
       <c r="I15" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="M15" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N15" s="32">
         <v>5</v>
       </c>
       <c r="O15" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B16" s="32">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G16" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H16" s="32">
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="M16" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N16" s="32">
         <v>6</v>
       </c>
       <c r="O16" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B17" s="32">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G17" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H17" s="32">
         <v>7</v>
       </c>
       <c r="I17" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="M17" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N17" s="32">
         <v>7</v>
       </c>
       <c r="O17" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B18" s="32">
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G18" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H18" s="32">
         <v>8</v>
       </c>
       <c r="I18" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="M18" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N18" s="32">
         <v>8</v>
       </c>
       <c r="O18" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="B19" s="32">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G19" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H19" s="32">
         <v>9</v>
       </c>
       <c r="I19" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="M19" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="N19" s="32">
         <v>9</v>
       </c>
       <c r="O19" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B21" s="32">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G21" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H21" s="32">
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="M21" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N21" s="32">
         <v>1</v>
       </c>
       <c r="O21" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B22" s="32">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G22" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H22" s="32">
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="M22" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N22" s="32">
         <v>2</v>
       </c>
       <c r="O22" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B23" s="32">
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G23" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H23" s="32">
         <v>3</v>
       </c>
       <c r="I23" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="M23" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N23" s="32">
         <v>3</v>
       </c>
       <c r="O23" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B24" s="32">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G24" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H24" s="32">
         <v>4</v>
       </c>
       <c r="I24" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="M24" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N24" s="32">
         <v>4</v>
       </c>
       <c r="O24" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B25" s="32">
         <v>5</v>
       </c>
       <c r="C25" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G25" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H25" s="32">
         <v>5</v>
       </c>
       <c r="I25" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="M25" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N25" s="32">
         <v>5</v>
       </c>
       <c r="O25" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B26" s="32">
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="G26" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H26" s="32">
         <v>6</v>
       </c>
       <c r="I26" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="M26" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N26" s="32">
         <v>6</v>
       </c>
       <c r="O26" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B27" s="32">
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G27" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H27" s="32">
         <v>7</v>
       </c>
       <c r="I27" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="M27" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N27" s="32">
         <v>7</v>
       </c>
       <c r="O27" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B28" s="32">
         <v>8</v>
       </c>
       <c r="C28" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G28" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H28" s="32">
         <v>8</v>
       </c>
       <c r="I28" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="M28" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N28" s="32">
         <v>8</v>
       </c>
       <c r="O28" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="B29" s="32">
         <v>9</v>
       </c>
       <c r="C29" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="H29" s="69">
         <v>9</v>
       </c>
       <c r="I29" s="3"/>
       <c r="M29" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="N29" s="32">
         <v>9</v>
       </c>
       <c r="O29" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B31" s="32">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="G31" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H31" s="32">
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N31" s="32">
         <v>1</v>
@@ -7949,22 +7960,22 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B32" s="32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G32" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H32" s="32">
         <v>2</v>
       </c>
       <c r="I32" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N32" s="32">
         <v>2</v>
@@ -7972,22 +7983,22 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B33" s="32">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="G33" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H33" s="32">
         <v>3</v>
       </c>
       <c r="I33" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N33" s="32">
         <v>3</v>
@@ -7995,22 +8006,22 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B34" s="32">
         <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G34" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H34" s="32">
         <v>4</v>
       </c>
       <c r="I34" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N34" s="32">
         <v>4</v>
@@ -8018,22 +8029,22 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B35" s="32">
         <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G35" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H35" s="32">
         <v>5</v>
       </c>
       <c r="I35" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N35" s="32">
         <v>5</v>
@@ -8041,22 +8052,22 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B36" s="32">
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G36" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H36" s="32">
         <v>6</v>
       </c>
       <c r="I36" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N36" s="32">
         <v>6</v>
@@ -8064,22 +8075,22 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B37" s="32">
         <v>7</v>
       </c>
       <c r="C37" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="G37" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H37" s="32">
         <v>7</v>
       </c>
       <c r="I37" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N37" s="32">
         <v>7</v>
@@ -8087,20 +8098,20 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B38" s="69">
         <v>8</v>
       </c>
       <c r="C38" s="3"/>
       <c r="G38" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H38" s="32">
         <v>8</v>
       </c>
       <c r="I38" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="N38" s="32">
         <v>8</v>
@@ -8108,14 +8119,14 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="B39" s="69">
         <v>9</v>
       </c>
       <c r="C39" s="3"/>
       <c r="G39" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="H39" s="32">
         <v>9</v>
@@ -8313,7 +8324,7 @@
         <v>451</v>
       </c>
       <c r="P10" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
@@ -8321,10 +8332,10 @@
         <v>452</v>
       </c>
       <c r="L11" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="P11" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.25">
@@ -8332,10 +8343,10 @@
         <v>453</v>
       </c>
       <c r="L12" t="s">
+        <v>654</v>
+      </c>
+      <c r="P12" t="s">
         <v>656</v>
-      </c>
-      <c r="P12" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
@@ -8366,14 +8377,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="140" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="137"/>
+      <c r="B1" s="141"/>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="142"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
@@ -8384,16 +8395,16 @@
       <c r="F2" s="22"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="138" t="s">
+      <c r="A3" s="143" t="s">
         <v>317</v>
       </c>
-      <c r="B3" s="139"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="138" t="s">
+      <c r="B3" s="144"/>
+      <c r="C3" s="145"/>
+      <c r="D3" s="143" t="s">
         <v>318</v>
       </c>
-      <c r="E3" s="139"/>
-      <c r="F3" s="140"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="145"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="23">
@@ -8650,8 +8661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8663,12 +8674,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="141" t="s">
-        <v>573</v>
-      </c>
-      <c r="B1" s="141"/>
-      <c r="C1" s="141"/>
-      <c r="D1" s="141"/>
+      <c r="A1" s="146" t="s">
+        <v>764</v>
+      </c>
+      <c r="B1" s="146"/>
+      <c r="C1" s="146"/>
+      <c r="D1" s="146"/>
       <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
@@ -8794,7 +8805,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="111" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="C10" s="109" t="s">
         <v>135</v>
@@ -8809,7 +8820,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="111" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="C11" s="109" t="s">
         <v>268</v>
@@ -8861,7 +8872,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
@@ -8876,31 +8887,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="173" t="s">
-        <v>763</v>
-      </c>
-      <c r="B1" s="173"/>
-      <c r="C1" s="173"/>
-      <c r="D1" s="173"/>
-      <c r="E1" s="173"/>
-      <c r="F1" s="173"/>
-      <c r="G1" s="173"/>
-      <c r="H1" s="173"/>
+      <c r="A1" s="150" t="s">
+        <v>761</v>
+      </c>
+      <c r="B1" s="150"/>
+      <c r="C1" s="150"/>
+      <c r="D1" s="150"/>
+      <c r="E1" s="150"/>
+      <c r="F1" s="150"/>
+      <c r="G1" s="150"/>
+      <c r="H1" s="150"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="147" t="s">
         <v>325</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="146"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="149"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="174" t="s">
+      <c r="A3" s="130" t="s">
         <v>326</v>
       </c>
       <c r="B3" s="104" t="s">
@@ -8912,7 +8923,7 @@
       <c r="D3" s="104" t="s">
         <v>302</v>
       </c>
-      <c r="E3" s="175" t="s">
+      <c r="E3" s="131" t="s">
         <v>326</v>
       </c>
       <c r="F3" s="104" t="s">
@@ -8930,10 +8941,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="106" t="s">
+        <v>612</v>
+      </c>
+      <c r="C4" s="106" t="s">
         <v>613</v>
-      </c>
-      <c r="C4" s="106" t="s">
-        <v>614</v>
       </c>
       <c r="D4" s="106"/>
       <c r="E4" s="104">
@@ -8954,17 +8965,17 @@
         <v>2</v>
       </c>
       <c r="B5" s="106" t="s">
+        <v>614</v>
+      </c>
+      <c r="C5" s="106" t="s">
         <v>615</v>
-      </c>
-      <c r="C5" s="106" t="s">
-        <v>616</v>
       </c>
       <c r="D5" s="106"/>
       <c r="E5" s="104">
         <v>12</v>
       </c>
       <c r="F5" s="106" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="G5" s="106" t="s">
         <v>58</v>
@@ -8978,17 +8989,17 @@
         <v>3</v>
       </c>
       <c r="B6" s="106" t="s">
+        <v>616</v>
+      </c>
+      <c r="C6" s="106" t="s">
         <v>617</v>
-      </c>
-      <c r="C6" s="106" t="s">
-        <v>618</v>
       </c>
       <c r="D6" s="106"/>
       <c r="E6" s="104">
         <v>13</v>
       </c>
       <c r="F6" s="106" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G6" s="106" t="s">
         <v>269</v>
@@ -9002,7 +9013,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="106" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C7" s="106" t="s">
         <v>42</v>
@@ -9014,13 +9025,13 @@
         <v>14</v>
       </c>
       <c r="F7" s="106" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G7" s="106" t="s">
         <v>94</v>
       </c>
       <c r="H7" s="106" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -9028,7 +9039,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="106" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="C8" s="106" t="s">
         <v>113</v>
@@ -9052,7 +9063,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="106" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="C9" s="106" t="s">
         <v>128</v>
@@ -9064,7 +9075,7 @@
         <v>16</v>
       </c>
       <c r="F9" s="106" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G9" s="106" t="s">
         <v>546</v>
@@ -9088,7 +9099,7 @@
         <v>17</v>
       </c>
       <c r="F10" s="106" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G10" s="106" t="s">
         <v>117</v>
@@ -9102,7 +9113,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="106" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="C11" s="106" t="s">
         <v>41</v>
@@ -9128,7 +9139,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="106" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="C12" s="106" t="s">
         <v>120</v>
@@ -9184,16 +9195,16 @@
       <c r="H14" s="29"/>
     </row>
     <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="144" t="s">
+      <c r="A15" s="147" t="s">
         <v>327</v>
       </c>
-      <c r="B15" s="145"/>
-      <c r="C15" s="145"/>
-      <c r="D15" s="146"/>
+      <c r="B15" s="148"/>
+      <c r="C15" s="148"/>
+      <c r="D15" s="149"/>
       <c r="E15"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="174" t="s">
+      <c r="A16" s="130" t="s">
         <v>326</v>
       </c>
       <c r="B16" s="104" t="s">
@@ -9211,13 +9222,13 @@
       <c r="A17" s="104">
         <v>1</v>
       </c>
-      <c r="B17" s="176" t="s">
+      <c r="B17" s="132" t="s">
         <v>566</v>
       </c>
-      <c r="C17" s="177" t="s">
+      <c r="C17" s="133" t="s">
         <v>560</v>
       </c>
-      <c r="D17" s="176" t="s">
+      <c r="D17" s="132" t="s">
         <v>561</v>
       </c>
       <c r="E17"/>
@@ -9226,13 +9237,13 @@
       <c r="A18" s="104">
         <v>2</v>
       </c>
-      <c r="B18" s="176" t="s">
+      <c r="B18" s="132" t="s">
         <v>567</v>
       </c>
-      <c r="C18" s="177" t="s">
+      <c r="C18" s="133" t="s">
         <v>460</v>
       </c>
-      <c r="D18" s="177" t="s">
+      <c r="D18" s="133" t="s">
         <v>481</v>
       </c>
       <c r="E18"/>
@@ -9241,13 +9252,13 @@
       <c r="A19" s="104">
         <v>3</v>
       </c>
-      <c r="B19" s="176" t="s">
+      <c r="B19" s="132" t="s">
         <v>568</v>
       </c>
-      <c r="C19" s="177" t="s">
+      <c r="C19" s="133" t="s">
         <v>461</v>
       </c>
-      <c r="D19" s="177" t="s">
+      <c r="D19" s="133" t="s">
         <v>484</v>
       </c>
       <c r="E19"/>
@@ -9256,13 +9267,13 @@
       <c r="A20" s="104">
         <v>4</v>
       </c>
-      <c r="B20" s="176" t="s">
+      <c r="B20" s="132" t="s">
         <v>569</v>
       </c>
-      <c r="C20" s="177" t="s">
+      <c r="C20" s="133" t="s">
         <v>462</v>
       </c>
-      <c r="D20" s="177" t="s">
+      <c r="D20" s="133" t="s">
         <v>485</v>
       </c>
       <c r="E20"/>
@@ -9271,13 +9282,13 @@
       <c r="A21" s="104">
         <v>5</v>
       </c>
-      <c r="B21" s="176" t="s">
+      <c r="B21" s="132" t="s">
         <v>570</v>
       </c>
-      <c r="C21" s="177" t="s">
+      <c r="C21" s="133" t="s">
         <v>283</v>
       </c>
-      <c r="D21" s="177" t="s">
+      <c r="D21" s="133" t="s">
         <v>487</v>
       </c>
       <c r="E21"/>
@@ -9286,13 +9297,13 @@
       <c r="A22" s="104">
         <v>6</v>
       </c>
-      <c r="B22" s="176" t="s">
+      <c r="B22" s="132" t="s">
         <v>571</v>
       </c>
-      <c r="C22" s="177" t="s">
+      <c r="C22" s="133" t="s">
         <v>284</v>
       </c>
-      <c r="D22" s="177" t="s">
+      <c r="D22" s="133" t="s">
         <v>489</v>
       </c>
       <c r="E22"/>
@@ -9301,13 +9312,13 @@
       <c r="A23" s="104">
         <v>7</v>
       </c>
-      <c r="B23" s="176" t="s">
+      <c r="B23" s="132" t="s">
         <v>572</v>
       </c>
-      <c r="C23" s="177" t="s">
+      <c r="C23" s="133" t="s">
         <v>285</v>
       </c>
-      <c r="D23" s="177" t="s">
+      <c r="D23" s="133" t="s">
         <v>491</v>
       </c>
       <c r="E23"/>
@@ -9316,13 +9327,13 @@
       <c r="A24" s="104">
         <v>8</v>
       </c>
-      <c r="B24" s="176" t="s">
-        <v>760</v>
-      </c>
-      <c r="C24" s="177" t="s">
+      <c r="B24" s="132" t="s">
+        <v>758</v>
+      </c>
+      <c r="C24" s="133" t="s">
         <v>135</v>
       </c>
-      <c r="D24" s="177" t="s">
+      <c r="D24" s="133" t="s">
         <v>562</v>
       </c>
       <c r="E24"/>
@@ -9331,13 +9342,13 @@
       <c r="A25" s="104">
         <v>9</v>
       </c>
-      <c r="B25" s="176" t="s">
-        <v>761</v>
-      </c>
-      <c r="C25" s="177" t="s">
+      <c r="B25" s="132" t="s">
+        <v>759</v>
+      </c>
+      <c r="C25" s="133" t="s">
         <v>268</v>
       </c>
-      <c r="D25" s="177" t="s">
+      <c r="D25" s="133" t="s">
         <v>563</v>
       </c>
       <c r="E25"/>
@@ -9346,13 +9357,13 @@
       <c r="A26" s="104">
         <v>10</v>
       </c>
-      <c r="B26" s="176" t="s">
+      <c r="B26" s="132" t="s">
         <v>565</v>
       </c>
-      <c r="C26" s="177" t="s">
+      <c r="C26" s="133" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="177" t="s">
+      <c r="D26" s="133" t="s">
         <v>564</v>
       </c>
       <c r="E26"/>
@@ -9368,12 +9379,12 @@
       <c r="H27" s="29"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="144" t="s">
+      <c r="A28" s="147" t="s">
         <v>328</v>
       </c>
-      <c r="B28" s="145"/>
-      <c r="C28" s="145"/>
-      <c r="D28" s="146"/>
+      <c r="B28" s="148"/>
+      <c r="C28" s="148"/>
+      <c r="D28" s="149"/>
       <c r="E28"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
@@ -9396,13 +9407,13 @@
         <v>1</v>
       </c>
       <c r="B30" s="112" t="s">
+        <v>582</v>
+      </c>
+      <c r="C30" s="134" t="s">
         <v>583</v>
       </c>
-      <c r="C30" s="178" t="s">
+      <c r="D30" s="112" t="s">
         <v>584</v>
-      </c>
-      <c r="D30" s="112" t="s">
-        <v>585</v>
       </c>
       <c r="E30"/>
     </row>
@@ -9411,13 +9422,13 @@
         <v>2</v>
       </c>
       <c r="B31" s="112" t="s">
+        <v>585</v>
+      </c>
+      <c r="C31" s="134" t="s">
         <v>586</v>
       </c>
-      <c r="C31" s="178" t="s">
+      <c r="D31" s="112" t="s">
         <v>587</v>
-      </c>
-      <c r="D31" s="112" t="s">
-        <v>588</v>
       </c>
       <c r="E31"/>
     </row>
@@ -9426,13 +9437,13 @@
         <v>3</v>
       </c>
       <c r="B32" s="112" t="s">
+        <v>588</v>
+      </c>
+      <c r="C32" s="134" t="s">
         <v>589</v>
       </c>
-      <c r="C32" s="178" t="s">
+      <c r="D32" s="112" t="s">
         <v>590</v>
-      </c>
-      <c r="D32" s="112" t="s">
-        <v>591</v>
       </c>
       <c r="E32"/>
     </row>
@@ -9441,13 +9452,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="112" t="s">
+        <v>591</v>
+      </c>
+      <c r="C33" s="134" t="s">
         <v>592</v>
       </c>
-      <c r="C33" s="178" t="s">
+      <c r="D33" s="112" t="s">
         <v>593</v>
-      </c>
-      <c r="D33" s="112" t="s">
-        <v>594</v>
       </c>
       <c r="E33"/>
     </row>
@@ -9456,13 +9467,13 @@
         <v>5</v>
       </c>
       <c r="B34" s="112" t="s">
+        <v>594</v>
+      </c>
+      <c r="C34" s="134" t="s">
         <v>595</v>
       </c>
-      <c r="C34" s="178" t="s">
+      <c r="D34" s="112" t="s">
         <v>596</v>
-      </c>
-      <c r="D34" s="112" t="s">
-        <v>597</v>
       </c>
       <c r="E34"/>
     </row>
@@ -9471,13 +9482,13 @@
         <v>6</v>
       </c>
       <c r="B35" s="112" t="s">
+        <v>597</v>
+      </c>
+      <c r="C35" s="134" t="s">
         <v>598</v>
       </c>
-      <c r="C35" s="178" t="s">
+      <c r="D35" s="112" t="s">
         <v>599</v>
-      </c>
-      <c r="D35" s="112" t="s">
-        <v>600</v>
       </c>
       <c r="E35"/>
     </row>
@@ -9486,13 +9497,13 @@
         <v>7</v>
       </c>
       <c r="B36" s="112" t="s">
+        <v>600</v>
+      </c>
+      <c r="C36" s="134" t="s">
         <v>601</v>
       </c>
-      <c r="C36" s="178" t="s">
+      <c r="D36" s="112" t="s">
         <v>602</v>
-      </c>
-      <c r="D36" s="112" t="s">
-        <v>603</v>
       </c>
       <c r="E36"/>
     </row>
@@ -9501,13 +9512,13 @@
         <v>8</v>
       </c>
       <c r="B37" s="112" t="s">
+        <v>603</v>
+      </c>
+      <c r="C37" s="134" t="s">
         <v>604</v>
       </c>
-      <c r="C37" s="178" t="s">
+      <c r="D37" s="112" t="s">
         <v>605</v>
-      </c>
-      <c r="D37" s="112" t="s">
-        <v>606</v>
       </c>
       <c r="E37"/>
     </row>
@@ -9516,13 +9527,13 @@
         <v>9</v>
       </c>
       <c r="B38" s="112" t="s">
+        <v>606</v>
+      </c>
+      <c r="C38" s="134" t="s">
         <v>607</v>
       </c>
-      <c r="C38" s="178" t="s">
+      <c r="D38" s="112" t="s">
         <v>608</v>
-      </c>
-      <c r="D38" s="112" t="s">
-        <v>609</v>
       </c>
       <c r="E38"/>
     </row>
@@ -9531,13 +9542,13 @@
         <v>10</v>
       </c>
       <c r="B39" s="112" t="s">
+        <v>609</v>
+      </c>
+      <c r="C39" s="134" t="s">
         <v>610</v>
       </c>
-      <c r="C39" s="178" t="s">
+      <c r="D39" s="112" t="s">
         <v>611</v>
-      </c>
-      <c r="D39" s="112" t="s">
-        <v>612</v>
       </c>
       <c r="E39"/>
     </row>
@@ -9557,8 +9568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9575,28 +9586,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="142" t="s">
-        <v>644</v>
-      </c>
-      <c r="B1" s="142"/>
-      <c r="C1" s="142"/>
-      <c r="D1" s="142"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="142"/>
-      <c r="G1" s="142"/>
-      <c r="H1" s="142"/>
+      <c r="A1" s="151" t="s">
+        <v>763</v>
+      </c>
+      <c r="B1" s="151"/>
+      <c r="C1" s="151"/>
+      <c r="D1" s="151"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="151"/>
+      <c r="G1" s="151"/>
+      <c r="H1" s="151"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="144" t="s">
+      <c r="A2" s="147" t="s">
         <v>320</v>
       </c>
-      <c r="B2" s="145"/>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="145"/>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145"/>
-      <c r="H2" s="146"/>
+      <c r="B2" s="148"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="148"/>
+      <c r="E2" s="148"/>
+      <c r="F2" s="148"/>
+      <c r="G2" s="148"/>
+      <c r="H2" s="149"/>
     </row>
     <row r="3" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="103"/>
@@ -9625,7 +9636,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="113" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="C4" s="113"/>
       <c r="D4" s="106"/>
@@ -9659,7 +9670,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="113" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="C6" s="113" t="s">
         <v>547</v>
@@ -9677,7 +9688,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="113" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="C7" s="113">
         <v>121.3</v>
@@ -9695,10 +9706,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="113" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="C8" s="113" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="D8" s="106"/>
       <c r="E8" s="104">
@@ -9731,7 +9742,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="113" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="C10" s="113" t="s">
         <v>58</v>
@@ -9741,10 +9752,10 @@
         <v>17</v>
       </c>
       <c r="F10" s="113" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="G10" s="113" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="H10" s="113"/>
       <c r="M10" s="36"/>
@@ -9758,7 +9769,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="113" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="C11" s="113" t="s">
         <v>269</v>
@@ -9785,20 +9796,20 @@
         <v>9</v>
       </c>
       <c r="B12" s="113" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="C12" s="113" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D12" s="106"/>
       <c r="E12" s="104">
         <v>19</v>
       </c>
       <c r="F12" s="113" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="G12" s="113" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="H12" s="113"/>
       <c r="M12" s="36"/>
@@ -9818,10 +9829,10 @@
         <v>20</v>
       </c>
       <c r="F13" s="113" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="G13" s="113" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="H13" s="113"/>
       <c r="M13" s="36"/>
@@ -9831,16 +9842,16 @@
       <c r="Q13" s="36"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="144" t="s">
+      <c r="A14" s="147" t="s">
         <v>323</v>
       </c>
-      <c r="B14" s="147"/>
-      <c r="C14" s="147"/>
-      <c r="D14" s="147"/>
-      <c r="E14" s="147"/>
-      <c r="F14" s="147"/>
-      <c r="G14" s="147"/>
-      <c r="H14" s="148"/>
+      <c r="B14" s="153"/>
+      <c r="C14" s="153"/>
+      <c r="D14" s="153"/>
+      <c r="E14" s="153"/>
+      <c r="F14" s="153"/>
+      <c r="G14" s="153"/>
+      <c r="H14" s="154"/>
       <c r="M14" s="36"/>
       <c r="N14" s="36"/>
       <c r="O14" s="36"/>
@@ -9879,7 +9890,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="113" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="C16" s="113"/>
       <c r="D16" s="113"/>
@@ -9943,7 +9954,7 @@
         <v>109</v>
       </c>
       <c r="D18" s="113" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="E18" s="114">
         <v>13</v>
@@ -9986,7 +9997,7 @@
         <v>130</v>
       </c>
       <c r="H19" s="113" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="J19" s="36"/>
       <c r="K19" s="36"/>
@@ -10156,16 +10167,16 @@
       <c r="H25" s="113"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="144" t="s">
+      <c r="A26" s="147" t="s">
         <v>324</v>
       </c>
-      <c r="B26" s="147"/>
-      <c r="C26" s="147"/>
-      <c r="D26" s="147"/>
-      <c r="E26" s="147"/>
-      <c r="F26" s="147"/>
-      <c r="G26" s="147"/>
-      <c r="H26" s="148"/>
+      <c r="B26" s="153"/>
+      <c r="C26" s="153"/>
+      <c r="D26" s="153"/>
+      <c r="E26" s="153"/>
+      <c r="F26" s="153"/>
+      <c r="G26" s="153"/>
+      <c r="H26" s="154"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="103"/>
@@ -10212,7 +10223,7 @@
         <v>560</v>
       </c>
       <c r="H28" s="112" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -10232,7 +10243,7 @@
         <v>12</v>
       </c>
       <c r="F29" s="112" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G29" s="112" t="s">
         <v>460</v>
@@ -10258,7 +10269,7 @@
         <v>13</v>
       </c>
       <c r="F30" s="112" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="G30" s="112" t="s">
         <v>461</v>
@@ -10272,7 +10283,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="112" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C31" s="112" t="s">
         <v>200</v>
@@ -10284,7 +10295,7 @@
         <v>14</v>
       </c>
       <c r="F31" s="112" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="G31" s="112" t="s">
         <v>462</v>
@@ -10298,7 +10309,7 @@
         <v>5</v>
       </c>
       <c r="B32" s="112" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="C32" s="112" t="s">
         <v>226</v>
@@ -10310,7 +10321,7 @@
         <v>15</v>
       </c>
       <c r="F32" s="112" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="G32" s="112" t="s">
         <v>283</v>
@@ -10324,19 +10335,19 @@
         <v>6</v>
       </c>
       <c r="B33" s="112" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="C33" s="112" t="s">
         <v>204</v>
       </c>
       <c r="D33" s="112" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="E33" s="104">
         <v>16</v>
       </c>
       <c r="F33" s="112" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="G33" s="112" t="s">
         <v>284</v>
@@ -10350,19 +10361,19 @@
         <v>7</v>
       </c>
       <c r="B34" s="112" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="C34" s="112" t="s">
         <v>230</v>
       </c>
       <c r="D34" s="112" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E34" s="104">
         <v>17</v>
       </c>
       <c r="F34" s="112" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="G34" s="112" t="s">
         <v>285</v>
@@ -10376,13 +10387,13 @@
         <v>8</v>
       </c>
       <c r="B35" s="112" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="C35" s="112" t="s">
         <v>255</v>
       </c>
       <c r="D35" s="112" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="E35" s="104">
         <v>18</v>
@@ -10402,13 +10413,13 @@
         <v>9</v>
       </c>
       <c r="B36" s="112" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C36" s="112" t="s">
         <v>254</v>
       </c>
       <c r="D36" s="112" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="E36" s="104">
         <v>19</v>
@@ -10428,19 +10439,19 @@
         <v>10</v>
       </c>
       <c r="B37" s="112" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="C37" s="112" t="s">
         <v>177</v>
       </c>
       <c r="D37" s="112" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E37" s="104">
         <v>20</v>
       </c>
       <c r="F37" s="112" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="G37" s="112" t="s">
         <v>167</v>
@@ -10450,10 +10461,10 @@
       </c>
     </row>
     <row r="41" spans="1:9" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="B41" s="143"/>
-      <c r="C41" s="143"/>
-      <c r="D41" s="143"/>
-      <c r="E41" s="143"/>
+      <c r="B41" s="152"/>
+      <c r="C41" s="152"/>
+      <c r="D41" s="152"/>
+      <c r="E41" s="152"/>
       <c r="F41" s="123"/>
       <c r="G41" s="123"/>
       <c r="H41" s="123"/>
@@ -10694,40 +10705,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="149" t="s">
-        <v>751</v>
-      </c>
-      <c r="B1" s="150"/>
-      <c r="C1" s="150"/>
-      <c r="D1" s="150"/>
-      <c r="E1" s="150"/>
-      <c r="F1" s="150"/>
-      <c r="G1" s="150"/>
-      <c r="H1" s="151"/>
+      <c r="A1" s="155" t="s">
+        <v>749</v>
+      </c>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
+      <c r="F1" s="156"/>
+      <c r="G1" s="156"/>
+      <c r="H1" s="157"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="152"/>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="154"/>
+      <c r="A2" s="158"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="160"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="161" t="s">
         <v>398</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="155" t="s">
+      <c r="B3" s="162"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="161" t="s">
         <v>399</v>
       </c>
-      <c r="F3" s="156"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="158"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="164"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="88">
@@ -10737,7 +10748,7 @@
         <v>191</v>
       </c>
       <c r="C4" s="90" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D4" s="90" t="s">
         <v>400</v>
@@ -10750,7 +10761,7 @@
       </c>
       <c r="G4" s="74"/>
       <c r="H4" s="74" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10761,7 +10772,7 @@
         <v>262</v>
       </c>
       <c r="C5" s="90" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D5" s="90" t="s">
         <v>400</v>
@@ -10774,7 +10785,7 @@
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="74" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10785,7 +10796,7 @@
         <v>240</v>
       </c>
       <c r="C6" s="90" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D6" s="90" t="s">
         <v>400</v>
@@ -10798,7 +10809,7 @@
       </c>
       <c r="G6" s="74"/>
       <c r="H6" s="74" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10809,7 +10820,7 @@
         <v>259</v>
       </c>
       <c r="C7" s="90" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D7" s="90" t="s">
         <v>400</v>
@@ -10847,7 +10858,7 @@
         <v>109</v>
       </c>
       <c r="G8" s="74" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H8" s="74" t="s">
         <v>508</v>
@@ -10994,7 +11005,7 @@
         <v>533</v>
       </c>
       <c r="D14" s="90" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E14" s="88">
         <v>11</v>
@@ -11017,10 +11028,10 @@
         <v>256</v>
       </c>
       <c r="C15" s="90" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D15" s="90" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E15" s="88">
         <v>12</v>
@@ -11043,7 +11054,7 @@
         <v>245.75</v>
       </c>
       <c r="C16" s="90" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="D16" s="97" t="s">
         <v>344</v>
@@ -11069,7 +11080,7 @@
         <v>67</v>
       </c>
       <c r="C17" s="90" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="D17" s="97" t="s">
         <v>344</v>
@@ -11108,7 +11119,7 @@
       </c>
       <c r="G18" s="74"/>
       <c r="H18" s="74" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11132,7 +11143,7 @@
       </c>
       <c r="G19" s="74"/>
       <c r="H19" s="74" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11143,7 +11154,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="90" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D20" s="90" t="s">
         <v>555</v>
@@ -11156,7 +11167,7 @@
       </c>
       <c r="G20" s="74"/>
       <c r="H20" s="92" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11167,7 +11178,7 @@
         <v>241.75</v>
       </c>
       <c r="C21" s="74" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D21" s="74" t="s">
         <v>505</v>
@@ -11180,7 +11191,7 @@
       </c>
       <c r="G21" s="74"/>
       <c r="H21" s="92" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11228,7 +11239,7 @@
       </c>
       <c r="G23" s="74"/>
       <c r="H23" s="74" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11240,13 +11251,13 @@
         <v>21</v>
       </c>
       <c r="F24" s="73" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="G24" s="74" t="s">
         <v>526</v>
       </c>
       <c r="H24" s="92" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11264,7 +11275,7 @@
         <v>529</v>
       </c>
       <c r="H25" s="92" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11428,40 +11439,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
-        <v>750</v>
-      </c>
-      <c r="B1" s="159"/>
-      <c r="C1" s="159"/>
-      <c r="D1" s="159"/>
-      <c r="E1" s="159"/>
-      <c r="F1" s="159"/>
-      <c r="G1" s="159"/>
-      <c r="H1" s="159"/>
+      <c r="A1" s="165" t="s">
+        <v>748</v>
+      </c>
+      <c r="B1" s="165"/>
+      <c r="C1" s="165"/>
+      <c r="D1" s="165"/>
+      <c r="E1" s="165"/>
+      <c r="F1" s="165"/>
+      <c r="G1" s="165"/>
+      <c r="H1" s="165"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="153"/>
-      <c r="B2" s="153"/>
-      <c r="C2" s="153"/>
-      <c r="D2" s="153"/>
-      <c r="E2" s="153"/>
-      <c r="F2" s="153"/>
-      <c r="G2" s="153"/>
-      <c r="H2" s="153"/>
+      <c r="A2" s="159"/>
+      <c r="B2" s="159"/>
+      <c r="C2" s="159"/>
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="159"/>
     </row>
     <row r="3" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A3" s="155" t="s">
+      <c r="A3" s="161" t="s">
         <v>398</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="155" t="s">
+      <c r="B3" s="162"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="164"/>
+      <c r="E3" s="161" t="s">
         <v>399</v>
       </c>
-      <c r="F3" s="156"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="158"/>
+      <c r="F3" s="162"/>
+      <c r="G3" s="163"/>
+      <c r="H3" s="164"/>
     </row>
     <row r="4" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="88">
@@ -11471,7 +11482,7 @@
         <v>191</v>
       </c>
       <c r="C4" s="74" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="D4" s="90" t="s">
         <v>400</v>
@@ -11484,7 +11495,7 @@
       </c>
       <c r="G4" s="74"/>
       <c r="H4" s="74" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11495,7 +11506,7 @@
         <v>262</v>
       </c>
       <c r="C5" s="74" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="D5" s="90" t="s">
         <v>400</v>
@@ -11508,7 +11519,7 @@
       </c>
       <c r="G5" s="74"/>
       <c r="H5" s="74" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11519,7 +11530,7 @@
         <v>240</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="D6" s="90" t="s">
         <v>400</v>
@@ -11532,7 +11543,7 @@
       </c>
       <c r="G6" s="74"/>
       <c r="H6" s="74" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11543,7 +11554,7 @@
         <v>259</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="D7" s="90" t="s">
         <v>400</v>
@@ -11581,7 +11592,7 @@
         <v>109</v>
       </c>
       <c r="G8" s="74" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="H8" s="74" t="s">
         <v>508</v>
@@ -11728,7 +11739,7 @@
         <v>533</v>
       </c>
       <c r="D14" s="74" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="E14" s="88">
         <v>11</v>
@@ -11751,10 +11762,10 @@
         <v>256</v>
       </c>
       <c r="C15" s="74" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="D15" s="74" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E15" s="88">
         <v>12</v>
@@ -11780,7 +11791,7 @@
         <v>526</v>
       </c>
       <c r="D16" s="92" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E16" s="88">
         <v>13</v>
@@ -11806,7 +11817,7 @@
         <v>529</v>
       </c>
       <c r="D17" s="92" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E17" s="88">
         <v>14</v>
@@ -11842,7 +11853,7 @@
       </c>
       <c r="G18" s="74"/>
       <c r="H18" s="74" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11866,7 +11877,7 @@
       </c>
       <c r="G19" s="74"/>
       <c r="H19" s="74" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11877,7 +11888,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="74" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D20" s="74" t="s">
         <v>555</v>
@@ -11890,7 +11901,7 @@
       </c>
       <c r="G20" s="74"/>
       <c r="H20" s="92" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11901,7 +11912,7 @@
         <v>241.75</v>
       </c>
       <c r="C21" s="74" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="D21" s="74" t="s">
         <v>505</v>
@@ -11914,7 +11925,7 @@
       </c>
       <c r="G21" s="74"/>
       <c r="H21" s="92" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11962,7 +11973,7 @@
       </c>
       <c r="G23" s="74"/>
       <c r="H23" s="74" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
     </row>
   </sheetData>
@@ -11998,40 +12009,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="160" t="s">
-        <v>754</v>
-      </c>
-      <c r="B1" s="161"/>
-      <c r="C1" s="161"/>
-      <c r="D1" s="161"/>
-      <c r="E1" s="161"/>
-      <c r="F1" s="161"/>
-      <c r="G1" s="161"/>
-      <c r="H1" s="162"/>
+      <c r="A1" s="166" t="s">
+        <v>752</v>
+      </c>
+      <c r="B1" s="167"/>
+      <c r="C1" s="167"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
+      <c r="F1" s="167"/>
+      <c r="G1" s="167"/>
+      <c r="H1" s="168"/>
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="163"/>
-      <c r="B2" s="164"/>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
-      <c r="H2" s="165"/>
+      <c r="A2" s="169"/>
+      <c r="B2" s="170"/>
+      <c r="C2" s="170"/>
+      <c r="D2" s="170"/>
+      <c r="E2" s="170"/>
+      <c r="F2" s="170"/>
+      <c r="G2" s="170"/>
+      <c r="H2" s="171"/>
     </row>
     <row r="3" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="166" t="s">
-        <v>720</v>
-      </c>
-      <c r="B3" s="167"/>
-      <c r="C3" s="167"/>
-      <c r="D3" s="167"/>
-      <c r="E3" s="167" t="s">
-        <v>721</v>
-      </c>
-      <c r="F3" s="167"/>
-      <c r="G3" s="167"/>
-      <c r="H3" s="168"/>
+      <c r="A3" s="172" t="s">
+        <v>718</v>
+      </c>
+      <c r="B3" s="173"/>
+      <c r="C3" s="173"/>
+      <c r="D3" s="173"/>
+      <c r="E3" s="173" t="s">
+        <v>719</v>
+      </c>
+      <c r="F3" s="173"/>
+      <c r="G3" s="173"/>
+      <c r="H3" s="174"/>
     </row>
     <row r="4" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="71">
@@ -12040,7 +12051,7 @@
       <c r="B4" s="70"/>
       <c r="C4" s="70"/>
       <c r="D4" s="75" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E4" s="72">
         <v>1</v>
@@ -12048,7 +12059,7 @@
       <c r="F4" s="73"/>
       <c r="G4" s="74"/>
       <c r="H4" s="73" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12083,7 +12094,7 @@
         <v>109</v>
       </c>
       <c r="C6" s="74" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="D6" s="75" t="s">
         <v>508</v>
@@ -12096,7 +12107,7 @@
       </c>
       <c r="G6" s="74"/>
       <c r="H6" s="73" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12120,7 +12131,7 @@
       </c>
       <c r="G7" s="74"/>
       <c r="H7" s="73" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12140,11 +12151,11 @@
         <v>5</v>
       </c>
       <c r="F8" s="73" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G8" s="74"/>
       <c r="H8" s="73" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12196,7 +12207,7 @@
         <v>526</v>
       </c>
       <c r="H10" s="73" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12222,7 +12233,7 @@
         <v>529</v>
       </c>
       <c r="H11" s="73" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12242,11 +12253,11 @@
         <v>9</v>
       </c>
       <c r="F12" s="73" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="G12" s="74"/>
       <c r="H12" s="73" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12346,7 +12357,7 @@
         <v>130</v>
       </c>
       <c r="C17" s="74" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="D17" s="75" t="s">
         <v>555</v>
@@ -12409,11 +12420,11 @@
         <v>17</v>
       </c>
       <c r="F20" s="73" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="G20" s="74"/>
       <c r="H20" s="73" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12445,11 +12456,11 @@
         <v>19</v>
       </c>
       <c r="F22" s="73" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="G22" s="74"/>
       <c r="H22" s="73" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="18" x14ac:dyDescent="0.25">
@@ -12463,11 +12474,11 @@
         <v>20</v>
       </c>
       <c r="F23" s="128" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G23" s="129"/>
       <c r="H23" s="128" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated RAK twr to 121.6
</commit_message>
<xml_diff>
--- a/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
+++ b/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{525EA127-D150-48AB-BD7C-B9C8814DCA41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142192E8-D403-4E92-B4B2-696C654418AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35940" yWindow="6930" windowWidth="21600" windowHeight="12975" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1694" uniqueCount="764">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1693" uniqueCount="764">
   <si>
     <t>AWACS</t>
   </si>
@@ -3475,10 +3475,10 @@
     <xf numFmtId="49" fontId="22" fillId="19" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3948,7 +3948,7 @@
   <dimension ref="B3:AF51"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="O47" sqref="O47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4044,21 +4044,21 @@
       <c r="S4" s="30" t="s">
         <v>539</v>
       </c>
-      <c r="V4" s="135" t="s">
+      <c r="V4" s="136" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="135"/>
-      <c r="X4" s="135"/>
-      <c r="Z4" s="135" t="s">
+      <c r="W4" s="136"/>
+      <c r="X4" s="136"/>
+      <c r="Z4" s="136" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" s="135"/>
-      <c r="AB4" s="135"/>
-      <c r="AD4" s="135" t="s">
+      <c r="AA4" s="136"/>
+      <c r="AB4" s="136"/>
+      <c r="AD4" s="136" t="s">
         <v>292</v>
       </c>
-      <c r="AE4" s="135"/>
-      <c r="AF4" s="135"/>
+      <c r="AE4" s="136"/>
+      <c r="AF4" s="136"/>
     </row>
     <row r="5" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="51" t="s">
@@ -4537,11 +4537,11 @@
       <c r="X11" t="s">
         <v>509</v>
       </c>
-      <c r="Z11" s="135" t="s">
+      <c r="Z11" s="136" t="s">
         <v>19</v>
       </c>
-      <c r="AA11" s="135"/>
-      <c r="AB11" s="135"/>
+      <c r="AA11" s="136"/>
+      <c r="AB11" s="136"/>
     </row>
     <row r="12" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="51" t="s">
@@ -4968,11 +4968,11 @@
         <v>310</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="135" t="s">
+      <c r="R18" s="136" t="s">
         <v>2</v>
       </c>
-      <c r="S18" s="135"/>
-      <c r="T18" s="135"/>
+      <c r="S18" s="136"/>
+      <c r="T18" s="136"/>
     </row>
     <row r="19" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B19" s="51" t="s">
@@ -5035,13 +5035,13 @@
       <c r="X19" s="138"/>
       <c r="Y19" s="138"/>
       <c r="Z19" s="139"/>
-      <c r="AB19" s="135" t="s">
+      <c r="AB19" s="136" t="s">
         <v>14</v>
       </c>
-      <c r="AC19" s="135"/>
-      <c r="AD19" s="135"/>
-      <c r="AE19" s="135"/>
-      <c r="AF19" s="135"/>
+      <c r="AC19" s="136"/>
+      <c r="AD19" s="136"/>
+      <c r="AE19" s="136"/>
+      <c r="AF19" s="136"/>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B20" s="51" t="s">
@@ -5430,11 +5430,11 @@
       </c>
       <c r="O25" s="46"/>
       <c r="P25" s="4"/>
-      <c r="R25" s="135" t="s">
+      <c r="R25" s="136" t="s">
         <v>555</v>
       </c>
-      <c r="S25" s="135"/>
-      <c r="T25" s="135"/>
+      <c r="S25" s="136"/>
+      <c r="T25" s="136"/>
     </row>
     <row r="26" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B26" s="51" t="s">
@@ -5593,33 +5593,33 @@
       </c>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B31" s="135" t="s">
+      <c r="B31" s="136" t="s">
         <v>311</v>
       </c>
-      <c r="C31" s="135"/>
-      <c r="D31" s="135"/>
-      <c r="E31" s="135"/>
-      <c r="F31" s="135"/>
-      <c r="G31" s="135"/>
-      <c r="H31" s="135"/>
-      <c r="J31" s="135" t="s">
+      <c r="C31" s="136"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="136"/>
+      <c r="F31" s="136"/>
+      <c r="G31" s="136"/>
+      <c r="H31" s="136"/>
+      <c r="J31" s="136" t="s">
         <v>312</v>
       </c>
-      <c r="K31" s="135"/>
-      <c r="L31" s="135"/>
-      <c r="M31" s="135"/>
-      <c r="N31" s="135"/>
-      <c r="O31" s="135"/>
-      <c r="P31" s="135"/>
-      <c r="U31" s="135" t="s">
+      <c r="K31" s="136"/>
+      <c r="L31" s="136"/>
+      <c r="M31" s="136"/>
+      <c r="N31" s="136"/>
+      <c r="O31" s="136"/>
+      <c r="P31" s="136"/>
+      <c r="U31" s="136" t="s">
         <v>294</v>
       </c>
-      <c r="V31" s="135"/>
-      <c r="W31" s="135"/>
-      <c r="X31" s="135"/>
-      <c r="Y31" s="135"/>
-      <c r="Z31" s="135"/>
-      <c r="AA31" s="135"/>
+      <c r="V31" s="136"/>
+      <c r="W31" s="136"/>
+      <c r="X31" s="136"/>
+      <c r="Y31" s="136"/>
+      <c r="Z31" s="136"/>
+      <c r="AA31" s="136"/>
     </row>
     <row r="32" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B32" s="45" t="s">
@@ -6068,15 +6068,15 @@
       <c r="F39" t="s">
         <v>633</v>
       </c>
-      <c r="J39" s="136" t="s">
+      <c r="J39" s="135" t="s">
         <v>492</v>
       </c>
-      <c r="K39" s="136"/>
-      <c r="L39" s="136"/>
-      <c r="M39" s="136"/>
-      <c r="N39" s="136"/>
-      <c r="O39" s="136"/>
-      <c r="P39" s="136"/>
+      <c r="K39" s="135"/>
+      <c r="L39" s="135"/>
+      <c r="M39" s="135"/>
+      <c r="N39" s="135"/>
+      <c r="O39" s="135"/>
+      <c r="P39" s="135"/>
       <c r="T39">
         <v>7</v>
       </c>
@@ -6299,11 +6299,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="U31:AA31"/>
-    <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="V19:Z19"/>
-    <mergeCell ref="J31:P31"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="R18:T18"/>
     <mergeCell ref="AB19:AF19"/>
@@ -6311,6 +6306,11 @@
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="R25:T25"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="U31:AA31"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="V19:Z19"/>
+    <mergeCell ref="J31:P31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9565,8 +9565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9828,8 +9828,8 @@
       <c r="F13" s="113" t="s">
         <v>755</v>
       </c>
-      <c r="G13" s="113" t="s">
-        <v>710</v>
+      <c r="G13" s="113">
+        <v>121.6</v>
       </c>
       <c r="H13" s="113"/>
       <c r="M13" s="36"/>
@@ -11991,7 +11991,7 @@
   </sheetPr>
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed tankers, updated tankers in CF file and updated tanker notam
</commit_message>
<xml_diff>
--- a/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
+++ b/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA81298B-C38C-4572-92EF-A0FAE779CF29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAAA0D40-3E21-4506-BE2E-7A995209038F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28365" yWindow="2865" windowWidth="21600" windowHeight="12975" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30345" yWindow="1860" windowWidth="21600" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -3499,10 +3499,10 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3974,8 +3974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:AF51"/>
   <sheetViews>
-    <sheetView topLeftCell="W1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AC42" sqref="AC42"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4071,21 +4071,21 @@
       <c r="S4" s="30" t="s">
         <v>539</v>
       </c>
-      <c r="V4" s="138" t="s">
+      <c r="V4" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="138"/>
-      <c r="X4" s="138"/>
-      <c r="Z4" s="138" t="s">
+      <c r="W4" s="139"/>
+      <c r="X4" s="139"/>
+      <c r="Z4" s="139" t="s">
         <v>18</v>
       </c>
-      <c r="AA4" s="138"/>
-      <c r="AB4" s="138"/>
-      <c r="AD4" s="138" t="s">
+      <c r="AA4" s="139"/>
+      <c r="AB4" s="139"/>
+      <c r="AD4" s="139" t="s">
         <v>292</v>
       </c>
-      <c r="AE4" s="138"/>
-      <c r="AF4" s="138"/>
+      <c r="AE4" s="139"/>
+      <c r="AF4" s="139"/>
     </row>
     <row r="5" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="51" t="s">
@@ -4409,7 +4409,7 @@
       <c r="G9" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="33" t="s">
+      <c r="H9" s="76" t="s">
         <v>89</v>
       </c>
       <c r="I9" s="34" t="s">
@@ -4564,11 +4564,11 @@
       <c r="X11" t="s">
         <v>509</v>
       </c>
-      <c r="Z11" s="138" t="s">
+      <c r="Z11" s="139" t="s">
         <v>19</v>
       </c>
-      <c r="AA11" s="138"/>
-      <c r="AB11" s="138"/>
+      <c r="AA11" s="139"/>
+      <c r="AB11" s="139"/>
     </row>
     <row r="12" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B12" s="51" t="s">
@@ -4659,7 +4659,7 @@
       <c r="G13" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="76" t="s">
         <v>455</v>
       </c>
       <c r="I13" s="16" t="s">
@@ -4995,11 +4995,11 @@
         <v>310</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="138" t="s">
+      <c r="R18" s="139" t="s">
         <v>2</v>
       </c>
-      <c r="S18" s="138"/>
-      <c r="T18" s="138"/>
+      <c r="S18" s="139"/>
+      <c r="T18" s="139"/>
     </row>
     <row r="19" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B19" s="51" t="s">
@@ -5062,13 +5062,13 @@
       <c r="X19" s="141"/>
       <c r="Y19" s="141"/>
       <c r="Z19" s="142"/>
-      <c r="AB19" s="138" t="s">
+      <c r="AB19" s="139" t="s">
         <v>14</v>
       </c>
-      <c r="AC19" s="138"/>
-      <c r="AD19" s="138"/>
-      <c r="AE19" s="138"/>
-      <c r="AF19" s="138"/>
+      <c r="AC19" s="139"/>
+      <c r="AD19" s="139"/>
+      <c r="AE19" s="139"/>
+      <c r="AF19" s="139"/>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B20" s="51" t="s">
@@ -5457,11 +5457,11 @@
       </c>
       <c r="O25" s="46"/>
       <c r="P25" s="4"/>
-      <c r="R25" s="138" t="s">
+      <c r="R25" s="139" t="s">
         <v>555</v>
       </c>
-      <c r="S25" s="138"/>
-      <c r="T25" s="138"/>
+      <c r="S25" s="139"/>
+      <c r="T25" s="139"/>
     </row>
     <row r="26" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B26" s="51" t="s">
@@ -5620,33 +5620,33 @@
       </c>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B31" s="138" t="s">
+      <c r="B31" s="139" t="s">
         <v>311</v>
       </c>
-      <c r="C31" s="138"/>
-      <c r="D31" s="138"/>
-      <c r="E31" s="138"/>
-      <c r="F31" s="138"/>
-      <c r="G31" s="138"/>
-      <c r="H31" s="138"/>
-      <c r="J31" s="138" t="s">
+      <c r="C31" s="139"/>
+      <c r="D31" s="139"/>
+      <c r="E31" s="139"/>
+      <c r="F31" s="139"/>
+      <c r="G31" s="139"/>
+      <c r="H31" s="139"/>
+      <c r="J31" s="139" t="s">
         <v>312</v>
       </c>
-      <c r="K31" s="138"/>
-      <c r="L31" s="138"/>
-      <c r="M31" s="138"/>
-      <c r="N31" s="138"/>
-      <c r="O31" s="138"/>
-      <c r="P31" s="138"/>
-      <c r="U31" s="138" t="s">
+      <c r="K31" s="139"/>
+      <c r="L31" s="139"/>
+      <c r="M31" s="139"/>
+      <c r="N31" s="139"/>
+      <c r="O31" s="139"/>
+      <c r="P31" s="139"/>
+      <c r="U31" s="139" t="s">
         <v>294</v>
       </c>
-      <c r="V31" s="138"/>
-      <c r="W31" s="138"/>
-      <c r="X31" s="138"/>
-      <c r="Y31" s="138"/>
-      <c r="Z31" s="138"/>
-      <c r="AA31" s="138"/>
+      <c r="V31" s="139"/>
+      <c r="W31" s="139"/>
+      <c r="X31" s="139"/>
+      <c r="Y31" s="139"/>
+      <c r="Z31" s="139"/>
+      <c r="AA31" s="139"/>
       <c r="AC31" s="143" t="s">
         <v>764</v>
       </c>
@@ -6136,15 +6136,15 @@
       <c r="F39" t="s">
         <v>633</v>
       </c>
-      <c r="J39" s="139" t="s">
+      <c r="J39" s="138" t="s">
         <v>492</v>
       </c>
-      <c r="K39" s="139"/>
-      <c r="L39" s="139"/>
-      <c r="M39" s="139"/>
-      <c r="N39" s="139"/>
-      <c r="O39" s="139"/>
-      <c r="P39" s="139"/>
+      <c r="K39" s="138"/>
+      <c r="L39" s="138"/>
+      <c r="M39" s="138"/>
+      <c r="N39" s="138"/>
+      <c r="O39" s="138"/>
+      <c r="P39" s="138"/>
       <c r="T39">
         <v>7</v>
       </c>
@@ -6367,12 +6367,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="J39:P39"/>
-    <mergeCell ref="U31:AA31"/>
-    <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="V19:Z19"/>
-    <mergeCell ref="J31:P31"/>
-    <mergeCell ref="AC31:AE31"/>
     <mergeCell ref="B31:H31"/>
     <mergeCell ref="R18:T18"/>
     <mergeCell ref="AB19:AF19"/>
@@ -6380,6 +6374,12 @@
     <mergeCell ref="V4:X4"/>
     <mergeCell ref="Z4:AB4"/>
     <mergeCell ref="R25:T25"/>
+    <mergeCell ref="J39:P39"/>
+    <mergeCell ref="U31:AA31"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="V19:Z19"/>
+    <mergeCell ref="J31:P31"/>
+    <mergeCell ref="AC31:AE31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -11487,7 +11487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added farp poodoo to CF
</commit_message>
<xml_diff>
--- a/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
+++ b/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C7EB40-FCC1-4EB7-B174-CF69B0F1036E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88935384-9119-4B28-A50F-CDF76DC16DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -3181,7 +3181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="218">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3594,6 +3594,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3606,9 +3609,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3735,6 +3735,7 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4075,7 +4076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AF51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="M1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
@@ -4091,11 +4092,11 @@
       </c>
       <c r="W2" s="138"/>
       <c r="X2" s="138"/>
-      <c r="Z2" s="171" t="s">
+      <c r="Z2" s="172" t="s">
         <v>732</v>
       </c>
-      <c r="AA2" s="172"/>
-      <c r="AB2" s="173"/>
+      <c r="AA2" s="173"/>
+      <c r="AB2" s="174"/>
     </row>
     <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="C3" s="53">
@@ -4220,11 +4221,11 @@
       <c r="AB4" s="137" t="s">
         <v>461</v>
       </c>
-      <c r="AD4" s="170" t="s">
+      <c r="AD4" s="171" t="s">
         <v>287</v>
       </c>
-      <c r="AE4" s="170"/>
-      <c r="AF4" s="170"/>
+      <c r="AE4" s="171"/>
+      <c r="AF4" s="171"/>
     </row>
     <row r="5" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="51" t="s">
@@ -5159,11 +5160,11 @@
         <v>305</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="170" t="s">
+      <c r="R18" s="171" t="s">
         <v>2</v>
       </c>
-      <c r="S18" s="170"/>
-      <c r="T18" s="170"/>
+      <c r="S18" s="171"/>
+      <c r="T18" s="171"/>
       <c r="Z18" s="137" t="s">
         <v>730</v>
       </c>
@@ -5228,20 +5229,20 @@
       <c r="T19" s="45" t="s">
         <v>296</v>
       </c>
-      <c r="V19" s="171" t="s">
+      <c r="V19" s="172" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="172"/>
-      <c r="X19" s="172"/>
-      <c r="Y19" s="172"/>
-      <c r="Z19" s="173"/>
-      <c r="AB19" s="170" t="s">
+      <c r="W19" s="173"/>
+      <c r="X19" s="173"/>
+      <c r="Y19" s="173"/>
+      <c r="Z19" s="174"/>
+      <c r="AB19" s="171" t="s">
         <v>14</v>
       </c>
-      <c r="AC19" s="170"/>
-      <c r="AD19" s="170"/>
-      <c r="AE19" s="170"/>
-      <c r="AF19" s="170"/>
+      <c r="AC19" s="171"/>
+      <c r="AD19" s="171"/>
+      <c r="AE19" s="171"/>
+      <c r="AF19" s="171"/>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B20" s="51" t="s">
@@ -5630,11 +5631,11 @@
       </c>
       <c r="O25" s="46"/>
       <c r="P25" s="4"/>
-      <c r="R25" s="170" t="s">
+      <c r="R25" s="171" t="s">
         <v>516</v>
       </c>
-      <c r="S25" s="170"/>
-      <c r="T25" s="170"/>
+      <c r="S25" s="171"/>
+      <c r="T25" s="171"/>
     </row>
     <row r="26" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B26" s="51" t="s">
@@ -5793,33 +5794,33 @@
       </c>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B31" s="170" t="s">
+      <c r="B31" s="171" t="s">
         <v>306</v>
       </c>
-      <c r="C31" s="170"/>
-      <c r="D31" s="170"/>
-      <c r="E31" s="170"/>
-      <c r="F31" s="170"/>
-      <c r="G31" s="170"/>
-      <c r="H31" s="170"/>
-      <c r="J31" s="170" t="s">
+      <c r="C31" s="171"/>
+      <c r="D31" s="171"/>
+      <c r="E31" s="171"/>
+      <c r="F31" s="171"/>
+      <c r="G31" s="171"/>
+      <c r="H31" s="171"/>
+      <c r="J31" s="171" t="s">
         <v>307</v>
       </c>
-      <c r="K31" s="170"/>
-      <c r="L31" s="170"/>
-      <c r="M31" s="170"/>
-      <c r="N31" s="170"/>
-      <c r="O31" s="170"/>
-      <c r="P31" s="170"/>
-      <c r="U31" s="170" t="s">
+      <c r="K31" s="171"/>
+      <c r="L31" s="171"/>
+      <c r="M31" s="171"/>
+      <c r="N31" s="171"/>
+      <c r="O31" s="171"/>
+      <c r="P31" s="171"/>
+      <c r="U31" s="171" t="s">
         <v>289</v>
       </c>
-      <c r="V31" s="170"/>
-      <c r="W31" s="170"/>
-      <c r="X31" s="170"/>
-      <c r="Y31" s="170"/>
-      <c r="Z31" s="170"/>
-      <c r="AA31" s="170"/>
+      <c r="V31" s="171"/>
+      <c r="W31" s="171"/>
+      <c r="X31" s="171"/>
+      <c r="Y31" s="171"/>
+      <c r="Z31" s="171"/>
+      <c r="AA31" s="171"/>
       <c r="AC31" s="175" t="s">
         <v>707</v>
       </c>
@@ -6309,15 +6310,15 @@
       <c r="F39" t="s">
         <v>591</v>
       </c>
-      <c r="J39" s="174" t="s">
+      <c r="J39" s="170" t="s">
         <v>456</v>
       </c>
-      <c r="K39" s="174"/>
-      <c r="L39" s="174"/>
-      <c r="M39" s="174"/>
-      <c r="N39" s="174"/>
-      <c r="O39" s="174"/>
-      <c r="P39" s="174"/>
+      <c r="K39" s="170"/>
+      <c r="L39" s="170"/>
+      <c r="M39" s="170"/>
+      <c r="N39" s="170"/>
+      <c r="O39" s="170"/>
+      <c r="P39" s="170"/>
       <c r="T39">
         <v>7</v>
       </c>
@@ -6554,17 +6555,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="AB19:AF19"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="J39:P39"/>
     <mergeCell ref="U31:AA31"/>
     <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="V19:Z19"/>
     <mergeCell ref="J31:P31"/>
     <mergeCell ref="AC31:AE31"/>
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="AB19:AF19"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8395,8 +8396,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C6:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8459,12 +8460,13 @@
       <c r="C15" s="169" t="s">
         <v>752</v>
       </c>
+      <c r="D15" s="7"/>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" s="169" t="s">
         <v>753</v>
       </c>
-      <c r="D16" s="7"/>
+      <c r="D16" s="217"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="169" t="s">

</xml_diff>

<commit_message>
updated ras al K freq
</commit_message>
<xml_diff>
--- a/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
+++ b/FILES/OP BLUE HARVEST Frequency and Callsign master list.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6842B7-119D-4B89-9BC4-52F80AA35DBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9132DCD8-4B7D-470D-AD55-BF8979A62A92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52380" yWindow="780" windowWidth="38700" windowHeight="15435" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="38700" windowHeight="15435" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frequencies" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1676" uniqueCount="759">
   <si>
     <t>AWACS</t>
   </si>
@@ -2221,9 +2221,6 @@
     <t>TACTICAL FREQS</t>
   </si>
   <si>
-    <t>F-16C presets OPBH V1.1</t>
-  </si>
-  <si>
     <t>Alert Frequency</t>
   </si>
   <si>
@@ -2236,9 +2233,6 @@
     <t>JACKAL SEC</t>
   </si>
   <si>
-    <t xml:space="preserve">A-10C presets  - OPBH v 1.1 </t>
-  </si>
-  <si>
     <t>MI-8 presets OPBH V1.1</t>
   </si>
   <si>
@@ -2303,6 +2297,12 @@
   </si>
   <si>
     <t>F-14 presets OPBH V1.2</t>
+  </si>
+  <si>
+    <t>A-10C presets  - OPBH v 1.2</t>
+  </si>
+  <si>
+    <t>F-16C presets OPBH V1.2</t>
   </si>
 </sst>
 </file>
@@ -3608,9 +3608,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3621,6 +3618,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4089,8 +4089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AF52"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I56" sqref="I56"/>
+    <sheetView topLeftCell="K1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O58" sqref="O58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4105,11 +4105,11 @@
       </c>
       <c r="W2" s="137"/>
       <c r="X2" s="137"/>
-      <c r="Z2" s="176" t="s">
+      <c r="Z2" s="175" t="s">
         <v>730</v>
       </c>
-      <c r="AA2" s="177"/>
-      <c r="AB2" s="178"/>
+      <c r="AA2" s="176"/>
+      <c r="AB2" s="177"/>
     </row>
     <row r="3" spans="2:32" x14ac:dyDescent="0.25">
       <c r="C3" s="53">
@@ -4234,11 +4234,11 @@
       <c r="AB4" s="136" t="s">
         <v>461</v>
       </c>
-      <c r="AD4" s="175" t="s">
+      <c r="AD4" s="174" t="s">
         <v>287</v>
       </c>
-      <c r="AE4" s="175"/>
-      <c r="AF4" s="175"/>
+      <c r="AE4" s="174"/>
+      <c r="AF4" s="174"/>
     </row>
     <row r="5" spans="2:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B5" s="51" t="s">
@@ -5173,11 +5173,11 @@
         <v>305</v>
       </c>
       <c r="Q18" s="4"/>
-      <c r="R18" s="175" t="s">
+      <c r="R18" s="174" t="s">
         <v>2</v>
       </c>
-      <c r="S18" s="175"/>
-      <c r="T18" s="175"/>
+      <c r="S18" s="174"/>
+      <c r="T18" s="174"/>
       <c r="Z18" s="136" t="s">
         <v>728</v>
       </c>
@@ -5242,20 +5242,20 @@
       <c r="T19" s="45" t="s">
         <v>296</v>
       </c>
-      <c r="V19" s="176" t="s">
+      <c r="V19" s="175" t="s">
         <v>1</v>
       </c>
-      <c r="W19" s="177"/>
-      <c r="X19" s="177"/>
-      <c r="Y19" s="177"/>
-      <c r="Z19" s="178"/>
-      <c r="AB19" s="175" t="s">
+      <c r="W19" s="176"/>
+      <c r="X19" s="176"/>
+      <c r="Y19" s="176"/>
+      <c r="Z19" s="177"/>
+      <c r="AB19" s="174" t="s">
         <v>14</v>
       </c>
-      <c r="AC19" s="175"/>
-      <c r="AD19" s="175"/>
-      <c r="AE19" s="175"/>
-      <c r="AF19" s="175"/>
+      <c r="AC19" s="174"/>
+      <c r="AD19" s="174"/>
+      <c r="AE19" s="174"/>
+      <c r="AF19" s="174"/>
     </row>
     <row r="20" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B20" s="51" t="s">
@@ -5644,11 +5644,11 @@
       </c>
       <c r="O25" s="46"/>
       <c r="P25" s="4"/>
-      <c r="R25" s="175" t="s">
+      <c r="R25" s="174" t="s">
         <v>516</v>
       </c>
-      <c r="S25" s="175"/>
-      <c r="T25" s="175"/>
+      <c r="S25" s="174"/>
+      <c r="T25" s="174"/>
     </row>
     <row r="26" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B26" s="51" t="s">
@@ -5789,7 +5789,7 @@
         <v>11</v>
       </c>
       <c r="R28" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="S28" t="s">
         <v>518</v>
@@ -5800,7 +5800,7 @@
     </row>
     <row r="29" spans="2:32" x14ac:dyDescent="0.25">
       <c r="R29" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="S29">
         <v>280.8</v>
@@ -5815,33 +5815,33 @@
       </c>
     </row>
     <row r="31" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B31" s="175" t="s">
+      <c r="B31" s="174" t="s">
         <v>306</v>
       </c>
-      <c r="C31" s="175"/>
-      <c r="D31" s="175"/>
-      <c r="E31" s="175"/>
-      <c r="F31" s="175"/>
-      <c r="G31" s="175"/>
-      <c r="H31" s="175"/>
-      <c r="J31" s="175" t="s">
+      <c r="C31" s="174"/>
+      <c r="D31" s="174"/>
+      <c r="E31" s="174"/>
+      <c r="F31" s="174"/>
+      <c r="G31" s="174"/>
+      <c r="H31" s="174"/>
+      <c r="J31" s="174" t="s">
         <v>307</v>
       </c>
-      <c r="K31" s="175"/>
-      <c r="L31" s="175"/>
-      <c r="M31" s="175"/>
-      <c r="N31" s="175"/>
-      <c r="O31" s="175"/>
-      <c r="P31" s="175"/>
-      <c r="U31" s="175" t="s">
+      <c r="K31" s="174"/>
+      <c r="L31" s="174"/>
+      <c r="M31" s="174"/>
+      <c r="N31" s="174"/>
+      <c r="O31" s="174"/>
+      <c r="P31" s="174"/>
+      <c r="U31" s="174" t="s">
         <v>289</v>
       </c>
-      <c r="V31" s="175"/>
-      <c r="W31" s="175"/>
-      <c r="X31" s="175"/>
-      <c r="Y31" s="175"/>
-      <c r="Z31" s="175"/>
-      <c r="AA31" s="175"/>
+      <c r="V31" s="174"/>
+      <c r="W31" s="174"/>
+      <c r="X31" s="174"/>
+      <c r="Y31" s="174"/>
+      <c r="Z31" s="174"/>
+      <c r="AA31" s="174"/>
       <c r="AC31" s="179" t="s">
         <v>705</v>
       </c>
@@ -6331,15 +6331,15 @@
       <c r="F39" t="s">
         <v>591</v>
       </c>
-      <c r="J39" s="174" t="s">
+      <c r="J39" s="178" t="s">
         <v>456</v>
       </c>
-      <c r="K39" s="174"/>
-      <c r="L39" s="174"/>
-      <c r="M39" s="174"/>
-      <c r="N39" s="174"/>
-      <c r="O39" s="174"/>
-      <c r="P39" s="174"/>
+      <c r="K39" s="178"/>
+      <c r="L39" s="178"/>
+      <c r="M39" s="178"/>
+      <c r="N39" s="178"/>
+      <c r="O39" s="178"/>
+      <c r="P39" s="178"/>
       <c r="T39">
         <v>7</v>
       </c>
@@ -6497,7 +6497,7 @@
         <v>698</v>
       </c>
       <c r="S46" s="134">
-        <v>118.2</v>
+        <v>121.7</v>
       </c>
       <c r="W46" t="s">
         <v>677</v>
@@ -6582,28 +6582,28 @@
         <v>210</v>
       </c>
       <c r="Y52" s="171" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="Z52" s="173" t="s">
         <v>88</v>
       </c>
       <c r="AA52" s="171" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B31:H31"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="AB19:AF19"/>
-    <mergeCell ref="R25:T25"/>
-    <mergeCell ref="Z2:AB2"/>
     <mergeCell ref="J39:P39"/>
     <mergeCell ref="U31:AA31"/>
     <mergeCell ref="AD4:AF4"/>
     <mergeCell ref="V19:Z19"/>
     <mergeCell ref="J31:P31"/>
     <mergeCell ref="AC31:AE31"/>
+    <mergeCell ref="B31:H31"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="AB19:AF19"/>
+    <mergeCell ref="R25:T25"/>
+    <mergeCell ref="Z2:AB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8445,71 +8445,71 @@
   <sheetData>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="168" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" s="168" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="D7" s="7"/>
     </row>
     <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="168" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="D8" s="7"/>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="168" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" s="168" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" s="168" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="D11" s="7"/>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12" s="168" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="D12" s="7"/>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C13" s="168" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="D13" s="7"/>
     </row>
     <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" s="168" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="D14" s="170"/>
     </row>
     <row r="15" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C15" s="168" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="D15" s="7"/>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" s="168" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="D16" s="169"/>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C17" s="168" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="D17" s="7"/>
     </row>
@@ -9047,7 +9047,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="190" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="B1" s="190"/>
       <c r="C1" s="190"/>
@@ -9729,8 +9729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q61"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="115" zoomScaleNormal="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9748,7 +9748,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="191" t="s">
-        <v>736</v>
+        <v>757</v>
       </c>
       <c r="B1" s="191"/>
       <c r="C1" s="191"/>
@@ -9993,7 +9993,7 @@
         <v>698</v>
       </c>
       <c r="G13" s="108">
-        <v>118.2</v>
+        <v>121.7</v>
       </c>
       <c r="H13" s="108"/>
       <c r="M13" s="36"/>
@@ -10186,7 +10186,7 @@
         <v>15</v>
       </c>
       <c r="F20" s="101" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G20" s="164">
         <v>33.5</v>
@@ -10220,7 +10220,7 @@
         <v>16</v>
       </c>
       <c r="F21" s="101" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G21" s="164">
         <v>38.5</v>
@@ -10254,7 +10254,7 @@
         <v>17</v>
       </c>
       <c r="F22" s="101" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G22" s="164">
         <v>33.75</v>
@@ -10891,7 +10891,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="195" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="B1" s="196"/>
       <c r="C1" s="196"/>
@@ -10942,7 +10942,7 @@
       </c>
       <c r="G4" s="166"/>
       <c r="H4" s="166" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10966,7 +10966,7 @@
       </c>
       <c r="G5" s="166"/>
       <c r="H5" s="166" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10990,7 +10990,7 @@
       </c>
       <c r="G6" s="166"/>
       <c r="H6" s="166" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11564,7 +11564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -11583,7 +11583,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="205" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="B1" s="205"/>
       <c r="C1" s="205"/>
@@ -11638,7 +11638,7 @@
       </c>
       <c r="G4" s="71"/>
       <c r="H4" s="71" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11662,7 +11662,7 @@
       </c>
       <c r="G5" s="71"/>
       <c r="H5" s="71" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11686,7 +11686,7 @@
       </c>
       <c r="G6" s="71"/>
       <c r="H6" s="71" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -12140,7 +12140,7 @@
   <dimension ref="A1:O56"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12155,7 +12155,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="208" t="s">
-        <v>731</v>
+        <v>758</v>
       </c>
       <c r="B1" s="209"/>
       <c r="C1" s="209"/>
@@ -12619,7 +12619,7 @@
         <v>466</v>
       </c>
       <c r="D22" s="151" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="E22" s="69">
         <v>19</v>
@@ -12648,8 +12648,8 @@
       <c r="E23" s="120">
         <v>20</v>
       </c>
-      <c r="F23" s="121" t="s">
-        <v>661</v>
+      <c r="F23" s="121">
+        <v>121.7</v>
       </c>
       <c r="G23" s="122"/>
       <c r="H23" s="121" t="s">

</xml_diff>